<commit_message>
Cambio de plantilla para cargue de asistencias
</commit_message>
<xml_diff>
--- a/src/assets/files/Plantilla para el cargue de asistencias.xlsx
+++ b/src/assets/files/Plantilla para el cargue de asistencias.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28200" windowHeight="12870" activeTab="1"/>
+    <workbookView windowWidth="28785" windowHeight="13095"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t>#</t>
   </si>
@@ -260,7 +260,7 @@
     <t>Grupo 1</t>
   </si>
   <si>
-    <t>LITORAL</t>
+    <t>Litoral</t>
   </si>
   <si>
     <t>Grupo 2</t>
@@ -294,6 +294,57 @@
   </si>
   <si>
     <t>Grupo 12</t>
+  </si>
+  <si>
+    <t>MARKETING - 3A</t>
+  </si>
+  <si>
+    <t>MARKETING - 3B</t>
+  </si>
+  <si>
+    <t>MARKETING - 3C</t>
+  </si>
+  <si>
+    <t>MARKETING - 4</t>
+  </si>
+  <si>
+    <t>P.A.S - A</t>
+  </si>
+  <si>
+    <t>P.A.S - B</t>
+  </si>
+  <si>
+    <t>P.A.S - C</t>
+  </si>
+  <si>
+    <t>P.A.S - D</t>
+  </si>
+  <si>
+    <t>P.P.D - 4</t>
+  </si>
+  <si>
+    <t>REDES - 4</t>
+  </si>
+  <si>
+    <t>S.S.T - A</t>
+  </si>
+  <si>
+    <t>S.S.T - B</t>
+  </si>
+  <si>
+    <t>S.S.T - C</t>
+  </si>
+  <si>
+    <t>WEB - 3A</t>
+  </si>
+  <si>
+    <t>WEB - 3B</t>
+  </si>
+  <si>
+    <t>WEB - 3C</t>
+  </si>
+  <si>
+    <t>WEB - 4</t>
   </si>
 </sst>
 </file>
@@ -301,12 +352,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,29 +397,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -383,15 +412,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -413,16 +441,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -438,15 +496,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -454,13 +520,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -475,22 +534,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -517,187 +561,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -763,17 +807,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -788,16 +826,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -826,6 +864,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -840,175 +904,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1031,6 +1075,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1380,636 +1427,636 @@
   <sheetPr/>
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="11.4285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="11.4285714285714" style="9"/>
-    <col min="2" max="2" width="33.8571428571429" style="9" customWidth="1"/>
-    <col min="3" max="3" width="54.7142857142857" style="9" customWidth="1"/>
-    <col min="4" max="4" width="63.5714285714286" style="9" customWidth="1"/>
-    <col min="5" max="5" width="23.5714285714286" style="9" customWidth="1"/>
-    <col min="6" max="6" width="11.4285714285714" style="9" customWidth="1"/>
-    <col min="7" max="7" width="11.4285714285714" style="9"/>
-    <col min="8" max="8" width="11.2857142857143" style="9" customWidth="1"/>
-    <col min="9" max="16384" width="11.4285714285714" style="9"/>
+    <col min="1" max="1" width="11.4285714285714" style="10"/>
+    <col min="2" max="2" width="33.8571428571429" style="10" customWidth="1"/>
+    <col min="3" max="3" width="54.7142857142857" style="10" customWidth="1"/>
+    <col min="4" max="4" width="63.5714285714286" style="10" customWidth="1"/>
+    <col min="5" max="5" width="23.5714285714286" style="10" customWidth="1"/>
+    <col min="6" max="6" width="11.4285714285714" style="10" customWidth="1"/>
+    <col min="7" max="7" width="11.4285714285714" style="10"/>
+    <col min="8" max="8" width="11.2857142857143" style="10" customWidth="1"/>
+    <col min="9" max="16384" width="11.4285714285714" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="10">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="10">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="10">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="10">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="10">
+      <c r="A6" s="11">
         <v>5</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="10">
+      <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="10">
+      <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="10">
+      <c r="A9" s="11">
         <v>8</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="10">
+      <c r="A10" s="11">
         <v>9</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="10">
+      <c r="A11" s="11">
         <v>10</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="10">
+      <c r="A12" s="11">
         <v>11</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="10">
+      <c r="A13" s="11">
         <v>12</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="10">
+      <c r="A14" s="11">
         <v>13</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="10">
+      <c r="A15" s="11">
         <v>14</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="10">
+      <c r="A16" s="11">
         <v>15</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="10">
+      <c r="A17" s="11">
         <v>16</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="10">
+      <c r="A18" s="11">
         <v>17</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="10">
+      <c r="A19" s="11">
         <v>18</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="10">
+      <c r="A20" s="11">
         <v>19</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="10">
+      <c r="A21" s="11">
         <v>20</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="10">
+      <c r="A22" s="11">
         <v>21</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="10">
+      <c r="A23" s="11">
         <v>22</v>
       </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="10">
+      <c r="A24" s="11">
         <v>23</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="10">
+      <c r="A25" s="11">
         <v>24</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="10">
+      <c r="A26" s="11">
         <v>25</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="10">
+      <c r="A27" s="11">
         <v>26</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="10">
+      <c r="A28" s="11">
         <v>27</v>
       </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="10">
+      <c r="A29" s="11">
         <v>28</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="10">
+      <c r="A30" s="11">
         <v>29</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="10">
+      <c r="A31" s="11">
         <v>30</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="10">
+      <c r="A32" s="11">
         <v>31</v>
       </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="10">
+      <c r="A33" s="11">
         <v>32</v>
       </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="10">
+      <c r="A34" s="11">
         <v>33</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="10">
+      <c r="A35" s="11">
         <v>34</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="10">
+      <c r="A36" s="11">
         <v>35</v>
       </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="10">
+      <c r="A37" s="11">
         <v>36</v>
       </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="10">
+      <c r="A38" s="11">
         <v>37</v>
       </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="10">
+      <c r="A39" s="11">
         <v>38</v>
       </c>
-      <c r="B39" s="10"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="10">
+      <c r="A40" s="11">
         <v>39</v>
       </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="10">
+      <c r="A41" s="11">
         <v>40</v>
       </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="10">
+      <c r="A42" s="11">
         <v>41</v>
       </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="10">
+      <c r="A43" s="11">
         <v>42</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="10">
+      <c r="A44" s="11">
         <v>43</v>
       </c>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="10"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="10">
+      <c r="A45" s="11">
         <v>44</v>
       </c>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="10">
+      <c r="A46" s="11">
         <v>45</v>
       </c>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="10">
+      <c r="A47" s="11">
         <v>46</v>
       </c>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
-      <c r="H47" s="10"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="10">
+      <c r="A48" s="11">
         <v>47</v>
       </c>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="10"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="10">
+      <c r="A49" s="11">
         <v>48</v>
       </c>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="10"/>
-      <c r="H49" s="10"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="10">
+      <c r="A50" s="11">
         <v>49</v>
       </c>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1">
@@ -2022,6 +2069,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B50">
       <formula1>validaciones!$A$1:$A$2</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H$1:H$1048576">
+      <formula1>"0,1"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C50">
       <formula1>validaciones!$B$1:$B$8</formula1>
     </dataValidation>
@@ -2030,9 +2080,6 @@
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR DE FECHA" error="Recuerda que solo puedes ingresar fechas en formato de fecha. Ejemplo:&#10;&#10;01/01/2022 o 01-01-2022" promptTitle="Fecha en Formato Fecha" prompt="Solo puedes ingresar fechas en formato de fecha. Ejemplo:&#10;&#10;01/01/2022 o 01-01-2022" sqref="G$1:G$1048576">
       <formula1>44562</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H$1:H$1048576">
-      <formula1>"0,1"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2044,10 +2091,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G90" sqref="G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2511,13 +2558,115 @@
       </c>
       <c r="E63" s="8"/>
     </row>
+    <row r="64" spans="4:5">
+      <c r="D64" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E64" s="8"/>
+    </row>
+    <row r="65" spans="4:5">
+      <c r="D65" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E65" s="8"/>
+    </row>
+    <row r="66" spans="4:5">
+      <c r="D66" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E66" s="8"/>
+    </row>
+    <row r="67" spans="4:5">
+      <c r="D67" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E67" s="8"/>
+    </row>
+    <row r="68" spans="4:5">
+      <c r="D68" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E68" s="8"/>
+    </row>
+    <row r="69" spans="4:5">
+      <c r="D69" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E69" s="8"/>
+    </row>
+    <row r="70" spans="4:5">
+      <c r="D70" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E70" s="8"/>
+    </row>
+    <row r="71" spans="4:5">
+      <c r="D71" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E71" s="8"/>
+    </row>
+    <row r="72" spans="4:5">
+      <c r="D72" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E72" s="8"/>
+    </row>
+    <row r="73" spans="4:5">
+      <c r="D73" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E73" s="8"/>
+    </row>
+    <row r="74" spans="4:5">
+      <c r="D74" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E74" s="8"/>
+    </row>
+    <row r="75" spans="4:5">
+      <c r="D75" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E75" s="8"/>
+    </row>
+    <row r="76" spans="4:5">
+      <c r="D76" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E76" s="8"/>
+    </row>
+    <row r="77" spans="4:5">
+      <c r="D77" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E77" s="8"/>
+    </row>
+    <row r="78" spans="4:5">
+      <c r="D78" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E78" s="8"/>
+    </row>
+    <row r="79" spans="4:5">
+      <c r="D79" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E79" s="8"/>
+    </row>
+    <row r="80" spans="4:5">
+      <c r="D80" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E80" s="8"/>
+    </row>
   </sheetData>
   <sortState ref="H1:H67">
     <sortCondition ref="H29:H67"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="E1:E51"/>
-    <mergeCell ref="E52:E63"/>
+    <mergeCell ref="E52:E80"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>